<commit_message>
Update app with new tabs, user guide, and new pdf
</commit_message>
<xml_diff>
--- a/www/DataCheckingErrorCodesAll.xlsx
+++ b/www/DataCheckingErrorCodesAll.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apamydavis\Documents\Rabies\Data checking\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD332559-30A4-4085-9DF0-F5B22E4ACB86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DB80DB-936B-49F6-BA00-DC8992095F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E84F5965-98E7-48BF-8D4F-7B75C69AEA61}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -159,9 +162,6 @@
     <t>Density study issue</t>
   </si>
   <si>
-    <t>N40</t>
-  </si>
-  <si>
     <t>The DATELASTORV you entered doesn’t match the ORV shapefile.  Please check your records and edit in MIS.</t>
   </si>
   <si>
@@ -325,9 +325,6 @@
   </si>
   <si>
     <t>N32</t>
-  </si>
-  <si>
-    <t>A tooth sample was taken but it has been &gt;365 days since collection and no age results are entered.  If you have them, please enter results.</t>
   </si>
   <si>
     <t>Tooth Results issue</t>
@@ -421,6 +418,12 @@
   </si>
   <si>
     <t>There is a mismatch between the RABIESVNA_IUML value and the RABIESVNAINTERPRET value.  Please check your RVNA results file and edit MIS.</t>
+  </si>
+  <si>
+    <t>N38</t>
+  </si>
+  <si>
+    <t>A tooth sample was taken but it has been &gt;365 days since collection and no age results or TTCC are entered.  If you have them, please enter results.</t>
   </si>
 </sst>
 </file>
@@ -893,10 +896,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8D68EAD-F2A4-4C18-8779-35724A46995C}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,335 +1101,336 @@
     </row>
     <row r="18" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B18" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B24" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B26" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B34" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C34" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>90</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>93</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="s">
         <v>120</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>121</v>
+        <v>41</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>95</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="94" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update app and error codes June 2022
</commit_message>
<xml_diff>
--- a/www/DataCheckingErrorCodesAll.xlsx
+++ b/www/DataCheckingErrorCodesAll.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apamydavis\Documents\Rabies\Data checking\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DA2AE7-B188-4328-A067-E18C47896795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACC6CC5-61B3-40B5-B306-58106D1EBD1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1725" yWindow="2265" windowWidth="14955" windowHeight="11385" xr2:uid="{E84F5965-98E7-48BF-8D4F-7B75C69AEA61}"/>
+    <workbookView xWindow="13845" yWindow="1260" windowWidth="14955" windowHeight="11385" xr2:uid="{E84F5965-98E7-48BF-8D4F-7B75C69AEA61}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="122">
   <si>
     <t>ErrorCode</t>
   </si>
@@ -421,6 +421,9 @@
   </si>
   <si>
     <t>Please fill in PROCESSED&lt;30DAYSAGO when MISTARGET is “INTENTIONAL” (for trapping).</t>
+  </si>
+  <si>
+    <t>Please fill in RECAPTURE when MISTARGET is “INTENTIONAL” (for trapping).</t>
   </si>
 </sst>
 </file>
@@ -898,8 +901,8 @@
   </sheetPr>
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,7 +1181,7 @@
         <v>55</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
Update app error N07
</commit_message>
<xml_diff>
--- a/www/DataCheckingErrorCodesAll.xlsx
+++ b/www/DataCheckingErrorCodesAll.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apamydavis\Documents\Rabies\Data checking\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACC6CC5-61B3-40B5-B306-58106D1EBD1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F68730D-AD35-4224-91E5-555E4F211902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13845" yWindow="1260" windowWidth="14955" windowHeight="11385" xr2:uid="{E84F5965-98E7-48BF-8D4F-7B75C69AEA61}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="11700" windowHeight="11385" xr2:uid="{E84F5965-98E7-48BF-8D4F-7B75C69AEA61}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="120">
   <si>
     <t>ErrorCode</t>
   </si>
@@ -114,9 +114,6 @@
     <t>N07</t>
   </si>
   <si>
-    <t>If METHOD is "HANDCAUGHT/GATHERED" then FATE must be "'DIED UNDER CARE" or "EUTHANIZED" or "FOUND DEAD" or "OTHER" or "RELEASED".  See "scenarios.pdf" (last tab in data checker app).</t>
-  </si>
-  <si>
     <t>N08</t>
   </si>
   <si>
@@ -160,9 +157,6 @@
   </si>
   <si>
     <t>Density study issue</t>
-  </si>
-  <si>
-    <t>The DATELASTORV you entered doesn’t match the ORV shapefile.  Please check your records and edit in MIS.</t>
   </si>
   <si>
     <t>ORV issue</t>
@@ -405,9 +399,6 @@
     <t>There is a mismatch between the RABIESVNA_IUML value and the RABIESVNAINTERPRET value.  Please check your RVNA results file and edit MIS.</t>
   </si>
   <si>
-    <t>N38</t>
-  </si>
-  <si>
     <t>A tooth sample was taken but it has been &gt;365 days since collection and no age results or TTCC are entered.  If you have them, please enter results.</t>
   </si>
   <si>
@@ -424,6 +415,9 @@
   </si>
   <si>
     <t>Please fill in RECAPTURE when MISTARGET is “INTENTIONAL” (for trapping).</t>
+  </si>
+  <si>
+    <t>If METHOD is "HANDCAUGHT/GATHERED" then FATE must be "'DIED UNDER CARE" or "EUTHANIZED" or "FOUND DEAD" or "RELEASED".  See "scenarios.pdf" (last tab in data checker app).</t>
   </si>
 </sst>
 </file>
@@ -899,10 +893,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,7 +1010,7 @@
         <v>24</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>25</v>
+        <v>119</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>23</v>
@@ -1024,10 +1018,10 @@
     </row>
     <row r="11" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>27</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>23</v>
@@ -1035,10 +1029,10 @@
     </row>
     <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>29</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>23</v>
@@ -1046,10 +1040,10 @@
     </row>
     <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>31</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>23</v>
@@ -1057,10 +1051,10 @@
     </row>
     <row r="14" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>33</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>23</v>
@@ -1068,10 +1062,10 @@
     </row>
     <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>35</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>23</v>
@@ -1079,10 +1073,10 @@
     </row>
     <row r="16" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>37</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>23</v>
@@ -1090,343 +1084,332 @@
     </row>
     <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="C17" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>50</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>61</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="8" t="s">
         <v>64</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="8" t="s">
         <v>67</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="8" t="s">
         <v>70</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>73</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>76</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="8" t="s">
         <v>81</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C36" s="8" t="s">
         <v>84</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" s="8" t="s">
         <v>87</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C39" s="8" t="s">
         <v>92</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C40" s="8" t="s">
         <v>95</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" s="8" t="s">
         <v>101</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" s="8" t="s">
         <v>104</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C44" s="8" t="s">
         <v>107</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C45" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B45" s="7" t="s">
+    </row>
+    <row r="46" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="B46" s="11" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>42</v>
+      <c r="C46" s="12" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update error codes for new N25a error
</commit_message>
<xml_diff>
--- a/www/DataCheckingErrorCodesAll.xlsx
+++ b/www/DataCheckingErrorCodesAll.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usdagcc-my.sharepoint.com/personal/amy_j_davis_usda_gov/Documents/Documents/Rabies/Data checking/www/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{6F68730D-AD35-4224-91E5-555E4F211902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BFE4678-382B-41A2-B429-A4867F063D5F}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{6F68730D-AD35-4224-91E5-555E4F211902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DA925BE-E308-401E-97D3-56B779B85741}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E84F5965-98E7-48BF-8D4F-7B75C69AEA61}"/>
   </bookViews>
@@ -423,10 +423,10 @@
     <t>N25a</t>
   </si>
   <si>
-    <t>This IDNUMBER has a FATE of "EUTHANIZED" and then is recaptured.</t>
-  </si>
-  <si>
     <t>ID/Fate issue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This IDNUMBER has a FATE of "EUTHANIZED" or "FOUND DEAD" or "DIED UNDER CARE" and then is recaptured. Please check your records and edit MIS. </t>
   </si>
 </sst>
 </file>
@@ -905,7 +905,7 @@
   <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C47" sqref="A1:C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1234,15 +1234,15 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>120</v>
       </c>
       <c r="B30" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" s="8" t="s">
         <v>121</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">

</xml_diff>